<commit_message>
added takecovidtest funciton and dailyreport functions
</commit_message>
<xml_diff>
--- a/Patholab/Python/Daily Report.xlsx
+++ b/Patholab/Python/Daily Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
   <si>
     <t>VANDANA SATHYAN</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>02:52 PM</t>
+  </si>
+  <si>
+    <t>RAJ SHUKLA</t>
+  </si>
+  <si>
+    <t>RT-PCR</t>
+  </si>
+  <si>
+    <t>09:03 PM</t>
   </si>
 </sst>
 </file>
@@ -645,7 +654,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1596,6 +1605,41 @@
         <v>99</v>
       </c>
     </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>1111142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>22093852093</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>500</v>
+      </c>
+      <c r="J28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created sendpdf and sendcovidreport functions
</commit_message>
<xml_diff>
--- a/Patholab/Python/Daily Report.xlsx
+++ b/Patholab/Python/Daily Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="108">
   <si>
     <t>VANDANA SATHYAN</t>
   </si>
@@ -323,6 +323,21 @@
   </si>
   <si>
     <t>09:03 PM</t>
+  </si>
+  <si>
+    <t>SHIJIN MATHEW</t>
+  </si>
+  <si>
+    <t>shijinmathew95@gmail.com</t>
+  </si>
+  <si>
+    <t>NIHAL TIWARI</t>
+  </si>
+  <si>
+    <t>23/03/2022</t>
+  </si>
+  <si>
+    <t>04:56 PM</t>
   </si>
 </sst>
 </file>
@@ -654,7 +669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1640,6 +1655,41 @@
         <v>102</v>
       </c>
     </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>1111143</v>
+      </c>
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>4235252352</v>
+      </c>
+      <c r="F29" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29">
+        <v>500</v>
+      </c>
+      <c r="J29" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>